<commit_message>
Practical Exercise 5 dan 6
</commit_message>
<xml_diff>
--- a/chooseProduct.xlsx
+++ b/chooseProduct.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download\Mitech\Cintya - Practical Exercise 4\Practical Exercise 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cintya Yossy Silvana\git\PracticalExercise4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Username</t>
   </si>
@@ -72,6 +72,21 @@
   </si>
   <si>
     <t>productName</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>postalCode</t>
+  </si>
+  <si>
+    <t>Cintya</t>
+  </si>
+  <si>
+    <t>Nainggolan</t>
   </si>
 </sst>
 </file>
@@ -432,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,9 +458,11 @@
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,8 +472,17 @@
       <c r="C1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -466,8 +492,17 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>12020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -475,7 +510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -483,7 +518,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -491,7 +526,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -499,7 +534,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -507,10 +542,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">

</xml_diff>